<commit_message>
Updated the excel sheet with the overview of the different notebooks
</commit_message>
<xml_diff>
--- a/notebooks/notebooks_overview.xlsx
+++ b/notebooks/notebooks_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Notebook</t>
   </si>
@@ -50,6 +50,27 @@
   </si>
   <si>
     <t>Trained on IMDB dataset</t>
+  </si>
+  <si>
+    <t>2_bert_sc_td_balance</t>
+  </si>
+  <si>
+    <t>100min</t>
+  </si>
+  <si>
+    <t>Traind on a rebelance IMDB dataset with 75% postive and 25% negative</t>
+  </si>
+  <si>
+    <t>The dataset is smaller then it needs to be</t>
+  </si>
+  <si>
+    <t>3_bert_sc_base</t>
+  </si>
+  <si>
+    <t>209min</t>
+  </si>
+  <si>
+    <t>Trained on a bert model that differs between lowercase and uppercase</t>
   </si>
 </sst>
 </file>
@@ -59,13 +80,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -76,7 +103,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -103,6 +130,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFc6c6c6"/>
       </left>
@@ -117,20 +151,70 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -140,58 +224,7 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,181 +534,211 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="18" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="19" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="18" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="20" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="20" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="20" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="21" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="20" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="21" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="20" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="22" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="22" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="20" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="11">
         <v>8</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10">
+      <c r="D3" s="12"/>
+      <c r="E3" s="11">
         <v>3</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="13">
         <v>0.9</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="13">
         <v>0.79</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="4"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="93" customFormat="1" s="15">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="16">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="16">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="17">
+        <v>0.87</v>
+      </c>
+      <c r="H4" s="17">
+        <v>0.78</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="22.5" customFormat="1" s="15">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="16">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="16">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.89</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0.79</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made a new fine-tuned model and updated the the excel overview
</commit_message>
<xml_diff>
--- a/notebooks/notebooks_overview.xlsx
+++ b/notebooks/notebooks_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Notebook</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>Trained on a bert model that differs between lowercase and uppercase</t>
+  </si>
+  <si>
+    <t>4_bert_sc_fine_tuned</t>
+  </si>
+  <si>
+    <t>2e-5</t>
+  </si>
+  <si>
+    <t>Classified another 100 reviews from the ww2 dataset and used them tof ine-tune the model</t>
+  </si>
+  <si>
+    <t>Also changed from 2 classes to three classes</t>
   </si>
 </sst>
 </file>
@@ -95,16 +107,16 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -155,76 +167,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,19 +540,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="20" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="21" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="20" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="21" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="20" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="22" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="22" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="20" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="19" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="20" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="20" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="19" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="21" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="21" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -614,7 +620,7 @@
       </c>
       <c r="J3" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="93" customFormat="1" s="15">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="87" customFormat="1" s="15">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -635,14 +641,14 @@
       <c r="H4" s="17">
         <v>0.78</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="22.5" customFormat="1" s="15">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="87" customFormat="1" s="15">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>16</v>
@@ -663,22 +669,36 @@
       <c r="H5" s="17">
         <v>0.79</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="15">
       <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="16"/>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="16">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="16">
+        <v>3</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="5"/>
+      <c r="H6" s="17">
+        <v>0.81</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="15">
       <c r="A7" s="5"/>
@@ -689,7 +709,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="15">
@@ -701,7 +721,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="15">
@@ -713,7 +733,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="15">
@@ -725,7 +745,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="15">
@@ -737,7 +757,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="18"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a new model using roBERTa, and updated the excel overview
</commit_message>
<xml_diff>
--- a/notebooks/notebooks_overview.xlsx
+++ b/notebooks/notebooks_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Notebook</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Also changed from 2 classes to three classes</t>
+  </si>
+  <si>
+    <t>5_bert_sc_roBERTa_fine_tuned</t>
+  </si>
+  <si>
+    <t>224min</t>
+  </si>
+  <si>
+    <t>Trained on roBERTa</t>
   </si>
 </sst>
 </file>
@@ -102,13 +111,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -167,22 +176,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -199,25 +205,25 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -540,16 +546,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="20" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="20" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="19" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="21" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="21" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="17" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="18" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="19" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="18" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="20" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="20" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -561,36 +567,36 @@
       <c r="F1" s="2"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
+      <c r="I1" s="1"/>
       <c r="J1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -599,166 +605,180 @@
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>8</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="11">
+      <c r="D3" s="11"/>
+      <c r="E3" s="10">
         <v>3</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <v>0.9</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>0.79</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="87" customFormat="1" s="15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
+      <c r="J3" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="87" customFormat="1" s="14">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>8</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="16">
+      <c r="D4" s="1"/>
+      <c r="E4" s="15">
         <v>3</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>0.87</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>0.78</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="87" customFormat="1" s="15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="87" customFormat="1" s="14">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>8</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="16">
+      <c r="D5" s="1"/>
+      <c r="E5" s="15">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="16">
         <v>0.89</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="16">
         <v>0.79</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="15">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
+      <c r="J5" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="114" customFormat="1" s="14">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>3</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17">
+      <c r="F6" s="1"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
         <v>0.81</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="15">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="15">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="15">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="15">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="50.25" customFormat="1" s="14">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="15">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="15">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0.89</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="14">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="14">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="14">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="14">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the excel overview sheet
</commit_message>
<xml_diff>
--- a/notebooks/notebooks_overview.xlsx
+++ b/notebooks/notebooks_overview.xlsx
@@ -64,7 +64,7 @@
     <t>The dataset is smaller then it needs to be</t>
   </si>
   <si>
-    <t>3_bert_sc_base</t>
+    <t>3_bert_sc_base_cased</t>
   </si>
   <si>
     <t>209min</t>
@@ -101,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,12 +112,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -181,7 +175,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -190,19 +184,19 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -706,7 +700,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="50.25" customFormat="1" s="14">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="33" customFormat="1" s="14">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Updated the excel overview
</commit_message>
<xml_diff>
--- a/notebooks/notebooks_overview.xlsx
+++ b/notebooks/notebooks_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Notebook</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>Trained on roBERTa</t>
+  </si>
+  <si>
+    <t>6_bert_uncased_vs_cased</t>
+  </si>
+  <si>
+    <t>29min</t>
+  </si>
+  <si>
+    <t>bert-uncased</t>
+  </si>
+  <si>
+    <t>Trained on a 60/20/20 split</t>
+  </si>
+  <si>
+    <t>bert-cased</t>
   </si>
 </sst>
 </file>
@@ -728,27 +743,57 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="14">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="15"/>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="15">
+        <v>8</v>
+      </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="E8" s="15">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0.9351</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="14">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="15"/>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="15">
+        <v>8</v>
+      </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="16"/>
+      <c r="E9" s="15">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0.93</v>
+      </c>
       <c r="H9" s="16"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="14">
       <c r="A10" s="1"/>

</xml_diff>